<commit_message>
create frequency tables and histograms with the lighthouse data
</commit_message>
<xml_diff>
--- a/statistical-analysis/Cumulative Layout Shift t-test.xlsx
+++ b/statistical-analysis/Cumulative Layout Shift t-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgray/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgray/lighthouse-audit/statistical-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E5DE74-FB20-8542-B23B-F5E1B27BED53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62753FF3-2939-C747-8715-CADC9E19E397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{BA93DC48-996C-124C-8125-77ADC35B3B62}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21220" xr2:uid="{BA93DC48-996C-124C-8125-77ADC35B3B62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Angular (score)</t>
   </si>
@@ -113,6 +135,18 @@
   </si>
   <si>
     <t>t Critical two-tail</t>
+  </si>
+  <si>
+    <t>Bins a</t>
+  </si>
+  <si>
+    <t>Freq a</t>
+  </si>
+  <si>
+    <t>Freq r</t>
+  </si>
+  <si>
+    <t>Bins r</t>
   </si>
 </sst>
 </file>
@@ -234,11 +268,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,6 +281,11 @@
     <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,6 +307,1999 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cumulative Layout Shift (Angular)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6867-F942-9B3D-983357ECC485}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1839003280"/>
+        <c:axId val="1839003680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1839003280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Bins (Limits)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1839003680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1839003680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1839003280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cumulative Layout Shift (React)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D13-2A4D-9E46-B49BB8C516D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1918186928"/>
+        <c:axId val="1828420320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1918186928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Bins (Limits)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1828420320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1828420320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1918186928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>29882</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>58484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>439697</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>165633</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97E96924-8DCA-76D8-9ABA-18AB9DE23405}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>808958</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>197223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>450370</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D94E512A-578A-5BCC-EEB8-4F224ED846AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,10 +2599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33064702-0E5C-7A4A-A871-8B027FA9347C}">
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="I14" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,383 +2618,533 @@
     <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="I1" s="14" t="s">
+      <c r="G1" s="5"/>
+      <c r="I1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="I2" s="15"/>
+      <c r="M1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="I2" s="10"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+      <c r="N2" s="11" cm="1">
+        <f t="array" ref="N2:N9">FREQUENCY(A2:A11, M2:M8)</f>
+        <v>6</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11" cm="1">
+        <f t="array" ref="Q2:Q9">FREQUENCY(B2:B11, P2:P8)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>0.64800000000000002</v>
       </c>
-      <c r="B3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="8">
         <v>0.25919999999999999</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="8">
         <v>6.1899999999999997E-2</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="11" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="M3" s="11">
+        <v>0.61</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11">
+        <v>0.61</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
         <v>0.64800000000000002</v>
       </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="7">
         <v>0.1058179568882333</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="7">
         <v>6.189999999999999E-2</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="8">
         <v>0.25919999999999999</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="8">
         <v>6.1899999999999997E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>0</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="M4" s="11">
+        <f>M3 + 0.01</f>
+        <v>0.62</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11">
+        <f>P3 + 0.01</f>
+        <v>0.62</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7">
         <v>0.61899999999999999</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="12">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="12">
-        <v>0</v>
-      </c>
-      <c r="I5" s="12" t="s">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="7">
         <v>0.1119744</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="7">
         <v>3.8316099999999992E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="M5" s="11">
+        <f t="shared" ref="M5:M6" si="0">M4 + 0.01</f>
+        <v>0.63</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11">
+        <f t="shared" ref="P5:P6" si="1">P4 + 0.01</f>
+        <v>0.63</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
         <v>0.64800000000000002</v>
       </c>
-      <c r="B6" s="7">
-        <v>0</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="B6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="13" t="s">
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="8">
         <v>10</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>0</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="M6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11">
+        <f t="shared" si="1"/>
+        <v>0.64</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7">
         <v>0</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="8">
         <v>0.33462576111232084</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="8">
         <v>0.19574498716442265</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="7">
         <v>7.5145249999999997E-2</v>
       </c>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>0</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="K7" s="7"/>
+      <c r="M7" s="11">
+        <f>M6 + 0.01</f>
+        <v>0.65</v>
+      </c>
+      <c r="N7" s="11">
+        <v>4</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11">
+        <f>P6 + 0.01</f>
+        <v>0.65</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>0</v>
+      </c>
+      <c r="B8" s="15">
         <v>0</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="7">
         <v>0.1119744</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="7">
         <v>3.8316099999999992E-2</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>0</v>
-      </c>
-      <c r="B9" s="8">
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="M8" s="11">
+        <f>M7 + 0.01</f>
+        <v>0.66</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11">
+        <f>P7 + 0.01</f>
+        <v>0.66</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7">
         <v>0</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="7">
         <v>-2.2767857142857149</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="7">
         <v>10.000000000000018</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="7">
         <v>18</v>
       </c>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>0</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="K9" s="7"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>0</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="7">
         <v>0.48412291827592746</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="7">
         <v>3.1622776601683822</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="7">
         <v>1.6093900819159388</v>
       </c>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="K10" s="7"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
         <v>0.64800000000000002</v>
       </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="7">
         <v>0.64800000000000002</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="7">
         <v>0.61899999999999999</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="8">
         <v>6.2464294062944986E-2</v>
       </c>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="K11" s="7"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12" t="s">
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="7">
         <v>1.7340636066175394</v>
       </c>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="K12" s="7"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="7">
         <v>0.64800000000000002</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="7">
         <v>0.61899999999999999</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="7">
         <v>0.12492858812588997</v>
       </c>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="K13" s="7"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+    </row>
+    <row r="14" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="7">
         <v>2.5920000000000001</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="7">
         <v>0.61899999999999999</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="7">
         <v>2.1009220402410378</v>
       </c>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="K14" s="7"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+    </row>
+    <row r="15" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="8">
         <v>10</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>
@@ -1241,5 +3418,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>